<commit_message>
Changes to be committed: 	modified:   Service status and description 2026.xlsx 	new file:   my_uconnect.py 	new file:   requirements.txt 	new file:   stellantis_client.py 	new file:   temp.json     new file:   temp.txt 	renamed:    temp -> temp1.json
</commit_message>
<xml_diff>
--- a/Service status and description 2026.xlsx
+++ b/Service status and description 2026.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{630FB211-D9B6-446C-9095-173638A278ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{B9778E1F-E5F6-4DAA-9339-D911909F943B}"/>
+    <workbookView xWindow="-23148" yWindow="1320" windowWidth="23256" windowHeight="13896" xr2:uid="{B9778E1F-E5F6-4DAA-9339-D911909F943B}"/>
   </bookViews>
   <sheets>
     <sheet name="JSON" sheetId="1" r:id="rId1"/>
@@ -1407,39 +1407,6 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1503,13 +1470,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="medium">
           <color rgb="FF000000"/>
         </left>
@@ -1519,6 +1479,13 @@
         <top style="medium">
           <color rgb="FF000000"/>
         </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1534,22 +1501,25 @@
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
         <charset val="238"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
+        <left style="medium">
           <color rgb="FF000000"/>
         </left>
-        <right style="thin">
+        <right style="medium">
           <color rgb="FF000000"/>
         </right>
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1664,13 +1634,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1683,6 +1646,43 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1699,7 +1699,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C067877-2382-47D7-B306-D95291580337}" name="Table1" displayName="Table1" ref="A1:D152" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C067877-2382-47D7-B306-D95291580337}" name="Table1" displayName="Table1" ref="A1:D152" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="A1:D152" xr:uid="{2C067877-2382-47D7-B306-D95291580337}">
     <filterColumn colId="1">
       <filters>
@@ -1708,10 +1708,10 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C537ABB2-0A9E-4786-B66F-E1DA2C3A0943}" name="ServiceCode" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{B6216EEF-84B0-4D95-A1FC-D7E4900295EA}" name="VehicleCapable" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{C4FB39DB-8A32-417D-97FA-DC148A372B47}" name="ServiceEnabled" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{1077C35D-D7F1-421D-BC7C-92A9F434C84F}" name="Service Description" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{C537ABB2-0A9E-4786-B66F-E1DA2C3A0943}" name="ServiceCode" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{B6216EEF-84B0-4D95-A1FC-D7E4900295EA}" name="VehicleCapable" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{C4FB39DB-8A32-417D-97FA-DC148A372B47}" name="ServiceEnabled" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{1077C35D-D7F1-421D-BC7C-92A9F434C84F}" name="Service Description" dataDxfId="5">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[ServiceCode]],Table2[#All],2,TRUE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1720,14 +1720,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1BCD0FF2-4E55-4A4C-8383-8C6E17F1ABBE}" name="Table2" displayName="Table2" ref="A1:B43" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="4" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1BCD0FF2-4E55-4A4C-8383-8C6E17F1ABBE}" name="Table2" displayName="Table2" ref="A1:B43" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
   <autoFilter ref="A1:B43" xr:uid="{1BCD0FF2-4E55-4A4C-8383-8C6E17F1ABBE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B43">
     <sortCondition ref="A1:A43"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{252D9ED2-E623-4A8B-86E9-A6E7C00DF84F}" name="Zkratka" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{A928E2B0-FDF8-43C7-96B2-D6CF25D0BC6E}" name="Pravděpodobný význam" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{252D9ED2-E623-4A8B-86E9-A6E7C00DF84F}" name="Zkratka" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{A928E2B0-FDF8-43C7-96B2-D6CF25D0BC6E}" name="Pravděpodobný význam" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2053,7 +2053,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2078,8 +2078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE7CB23-4A09-4CC9-A534-208BFA8DF60D}">
   <dimension ref="A1:D152"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection sqref="A1:D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>